<commit_message>
Inscription et nouveau logo
</commit_message>
<xml_diff>
--- a/public/html/budgetIkamu.xlsx
+++ b/public/html/budgetIkamu.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t xml:space="preserve">Dépense</t>
   </si>
@@ -47,13 +47,25 @@
     <t xml:space="preserve">Nourriture</t>
   </si>
   <si>
+    <t xml:space="preserve">Rallye Castor 2016</t>
+  </si>
+  <si>
     <t xml:space="preserve">Costumes</t>
   </si>
   <si>
+    <t xml:space="preserve">Rallye Branche Jaune</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brillant</t>
   </si>
   <si>
+    <t xml:space="preserve">CIME</t>
+  </si>
+  <si>
     <t xml:space="preserve">Camion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budget 10 ans</t>
   </si>
   <si>
     <t xml:space="preserve">Construction</t>
@@ -202,18 +214,15 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6071428571429"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.7857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.2959183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.3775510204082"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,11 +268,11 @@
       </c>
       <c r="G2" s="0" t="n">
         <f aca="false">SUM(F2:F1000)</f>
-        <v>14650</v>
+        <v>15450</v>
       </c>
       <c r="I2" s="0" t="n">
         <f aca="false">G2-C2</f>
-        <v>-200</v>
+        <v>600</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -274,34 +283,55 @@
         <f aca="false">SUM(JeunesCotisation!A2:A100)*JeunesCotisation!C2</f>
         <v>7050</v>
       </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>350</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>500</v>
       </c>
+      <c r="E4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="E5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>250</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>300</v>
       </c>
+      <c r="E6" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>300</v>
@@ -309,7 +339,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>500</v>
@@ -317,7 +347,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>100</v>
@@ -325,7 +355,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>500</v>
@@ -333,7 +363,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>200</v>
@@ -341,7 +371,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>300</v>
@@ -349,7 +379,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>200</v>
@@ -373,30 +403,30 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,7 +440,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,7 +454,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>